<commit_message>
Fixed bug 11: Edit profile
</commit_message>
<xml_diff>
--- a/_document/Bug Collectios.xlsx
+++ b/_document/Bug Collectios.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BQ96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Revision 200 :)) - Update File Bugcollection
</commit_message>
<xml_diff>
--- a/_document/Bug Collectios.xlsx
+++ b/_document/Bug Collectios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>1. Đưa group vào enable recommendation</t>
   </si>
@@ -376,7 +376,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -439,6 +439,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -863,7 +869,7 @@
   <dimension ref="A1:BQ96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1222,309 +1228,73 @@
       <c r="BP11" s="12"/>
       <c r="BQ11" s="12"/>
     </row>
-    <row r="12" spans="1:69">
-      <c r="A12">
+    <row r="12" spans="1:69" s="11" customFormat="1">
+      <c r="A12" s="11">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="12"/>
-      <c r="AA12" s="12"/>
-      <c r="AB12" s="12"/>
-      <c r="AC12" s="12"/>
-      <c r="AD12" s="12"/>
-      <c r="AE12" s="12"/>
-      <c r="AF12" s="12"/>
-      <c r="AG12" s="12"/>
-      <c r="AH12" s="12"/>
-      <c r="AI12" s="12"/>
-      <c r="AJ12" s="12"/>
-      <c r="AK12" s="12"/>
-      <c r="AL12" s="12"/>
-      <c r="AM12" s="12"/>
-      <c r="AN12" s="12"/>
-      <c r="AO12" s="12"/>
-      <c r="AP12" s="12"/>
-      <c r="AQ12" s="12"/>
-      <c r="AR12" s="12"/>
-      <c r="AS12" s="12"/>
-      <c r="AT12" s="12"/>
-      <c r="AU12" s="12"/>
-      <c r="AV12" s="12"/>
-      <c r="AW12" s="12"/>
-      <c r="AX12" s="12"/>
-      <c r="AY12" s="12"/>
-      <c r="AZ12" s="12"/>
-      <c r="BA12" s="12"/>
-      <c r="BB12" s="12"/>
-      <c r="BC12" s="12"/>
-      <c r="BD12" s="12"/>
-      <c r="BE12" s="12"/>
-      <c r="BF12" s="12"/>
-      <c r="BG12" s="12"/>
-      <c r="BH12" s="12"/>
-      <c r="BI12" s="12"/>
-      <c r="BJ12" s="12"/>
-      <c r="BK12" s="12"/>
-      <c r="BL12" s="12"/>
-      <c r="BM12" s="12"/>
-      <c r="BN12" s="12"/>
-      <c r="BO12" s="12"/>
-      <c r="BP12" s="12"/>
-      <c r="BQ12" s="12"/>
-    </row>
-    <row r="13" spans="1:69">
-      <c r="A13">
+      <c r="E12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69" s="11" customFormat="1">
+      <c r="A13" s="11">
         <v>9.1</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="12"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="12"/>
-      <c r="AF13" s="12"/>
-      <c r="AG13" s="12"/>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="12"/>
-      <c r="AJ13" s="12"/>
-      <c r="AK13" s="12"/>
-      <c r="AL13" s="12"/>
-      <c r="AM13" s="12"/>
-      <c r="AN13" s="12"/>
-      <c r="AO13" s="12"/>
-      <c r="AP13" s="12"/>
-      <c r="AQ13" s="12"/>
-      <c r="AR13" s="12"/>
-      <c r="AS13" s="12"/>
-      <c r="AT13" s="12"/>
-      <c r="AU13" s="12"/>
-      <c r="AV13" s="12"/>
-      <c r="AW13" s="12"/>
-      <c r="AX13" s="12"/>
-      <c r="AY13" s="12"/>
-      <c r="AZ13" s="12"/>
-      <c r="BA13" s="12"/>
-      <c r="BB13" s="12"/>
-      <c r="BC13" s="12"/>
-      <c r="BD13" s="12"/>
-      <c r="BE13" s="12"/>
-      <c r="BF13" s="12"/>
-      <c r="BG13" s="12"/>
-      <c r="BH13" s="12"/>
-      <c r="BI13" s="12"/>
-      <c r="BJ13" s="12"/>
-      <c r="BK13" s="12"/>
-      <c r="BL13" s="12"/>
-      <c r="BM13" s="12"/>
-      <c r="BN13" s="12"/>
-      <c r="BO13" s="12"/>
-      <c r="BP13" s="12"/>
-      <c r="BQ13" s="12"/>
-    </row>
-    <row r="14" spans="1:69">
-      <c r="A14">
+      <c r="E13" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69" s="11" customFormat="1">
+      <c r="A14" s="11">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="12"/>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="12"/>
-      <c r="AE14" s="12"/>
-      <c r="AF14" s="12"/>
-      <c r="AG14" s="12"/>
-      <c r="AH14" s="12"/>
-      <c r="AI14" s="12"/>
-      <c r="AJ14" s="12"/>
-      <c r="AK14" s="12"/>
-      <c r="AL14" s="12"/>
-      <c r="AM14" s="12"/>
-      <c r="AN14" s="12"/>
-      <c r="AO14" s="12"/>
-      <c r="AP14" s="12"/>
-      <c r="AQ14" s="12"/>
-      <c r="AR14" s="12"/>
-      <c r="AS14" s="12"/>
-      <c r="AT14" s="12"/>
-      <c r="AU14" s="12"/>
-      <c r="AV14" s="12"/>
-      <c r="AW14" s="12"/>
-      <c r="AX14" s="12"/>
-      <c r="AY14" s="12"/>
-      <c r="AZ14" s="12"/>
-      <c r="BA14" s="12"/>
-      <c r="BB14" s="12"/>
-      <c r="BC14" s="12"/>
-      <c r="BD14" s="12"/>
-      <c r="BE14" s="12"/>
-      <c r="BF14" s="12"/>
-      <c r="BG14" s="12"/>
-      <c r="BH14" s="12"/>
-      <c r="BI14" s="12"/>
-      <c r="BJ14" s="12"/>
-      <c r="BK14" s="12"/>
-      <c r="BL14" s="12"/>
-      <c r="BM14" s="12"/>
-      <c r="BN14" s="12"/>
-      <c r="BO14" s="12"/>
-      <c r="BP14" s="12"/>
-      <c r="BQ14" s="12"/>
-    </row>
-    <row r="15" spans="1:69">
-      <c r="A15">
+      <c r="E14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:69" s="11" customFormat="1">
+      <c r="A15" s="11">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="12"/>
-      <c r="AC15" s="12"/>
-      <c r="AD15" s="12"/>
-      <c r="AE15" s="12"/>
-      <c r="AF15" s="12"/>
-      <c r="AG15" s="12"/>
-      <c r="AH15" s="12"/>
-      <c r="AI15" s="12"/>
-      <c r="AJ15" s="12"/>
-      <c r="AK15" s="12"/>
-      <c r="AL15" s="12"/>
-      <c r="AM15" s="12"/>
-      <c r="AN15" s="12"/>
-      <c r="AO15" s="12"/>
-      <c r="AP15" s="12"/>
-      <c r="AQ15" s="12"/>
-      <c r="AR15" s="12"/>
-      <c r="AS15" s="12"/>
-      <c r="AT15" s="12"/>
-      <c r="AU15" s="12"/>
-      <c r="AV15" s="12"/>
-      <c r="AW15" s="12"/>
-      <c r="AX15" s="12"/>
-      <c r="AY15" s="12"/>
-      <c r="AZ15" s="12"/>
-      <c r="BA15" s="12"/>
-      <c r="BB15" s="12"/>
-      <c r="BC15" s="12"/>
-      <c r="BD15" s="12"/>
-      <c r="BE15" s="12"/>
-      <c r="BF15" s="12"/>
-      <c r="BG15" s="12"/>
-      <c r="BH15" s="12"/>
-      <c r="BI15" s="12"/>
-      <c r="BJ15" s="12"/>
-      <c r="BK15" s="12"/>
-      <c r="BL15" s="12"/>
-      <c r="BM15" s="12"/>
-      <c r="BN15" s="12"/>
-      <c r="BO15" s="12"/>
-      <c r="BP15" s="12"/>
-      <c r="BQ15" s="12"/>
+      <c r="E15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:69">
       <c r="A16">

</xml_diff>

<commit_message>
Fix toàn bộ lỗi notification - register wall post - xem liệt kê các chức năng có notification trong Bug Collectios.xlsx
</commit_message>
<xml_diff>
--- a/_document/Bug Collectios.xlsx
+++ b/_document/Bug Collectios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
   <si>
     <t>1. Đưa group vào enable recommendation</t>
   </si>
@@ -256,6 +256,75 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>Các thành phần notification &amp; wall post</t>
+  </si>
+  <si>
+    <t>notification</t>
+  </si>
+  <si>
+    <t>wall post</t>
+  </si>
+  <si>
+    <t>Add friends</t>
+  </si>
+  <si>
+    <t>Tag photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    notify khi add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   notify khi approve</t>
+  </si>
+  <si>
+    <t>notify khi tag photo</t>
+  </si>
+  <si>
+    <t>notify khi có người comment trên 1 bức ảnh có mình bên trong hoặc mình là chủ bức ảnh</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Topic comment okie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Notify cho những người đã comment trong topic đó khi có ng cm tiếp bên dưới</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Notify cho chủ topic khi có người cm</t>
+  </si>
+  <si>
+    <t>Invite to Group</t>
+  </si>
+  <si>
+    <t>notify khi accepted invitation</t>
+  </si>
+  <si>
+    <t>notify cho chủ nhóm khi một người join vào 1 nhóm thành công</t>
+  </si>
+  <si>
+    <t>notify cho chủ nhóm khi một người request để được vào nhóm</t>
+  </si>
+  <si>
+    <t>notify cho người request khi đã được chấp nhận</t>
+  </si>
+  <si>
+    <t>Hệ thống comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Notify cho người chủ topic biết khi có người comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Notify cho tất cả những người đã comment bên trên khi có cm mới</t>
+  </si>
+  <si>
+    <t>Notify khi viết testimony</t>
+  </si>
+  <si>
+    <t>Notify khi tag user( blog , poll)</t>
   </si>
 </sst>
 </file>
@@ -866,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BQ96"/>
+  <dimension ref="A1:BQ111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4976,7 +5045,7 @@
       <c r="BP80" s="12"/>
       <c r="BQ80" s="12"/>
     </row>
-    <row r="81" spans="5:69">
+    <row r="81" spans="2:69">
       <c r="E81" s="12"/>
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
@@ -5043,7 +5112,13 @@
       <c r="BP81" s="12"/>
       <c r="BQ81" s="12"/>
     </row>
-    <row r="82" spans="5:69">
+    <row r="82" spans="2:69">
+      <c r="C82" t="s">
+        <v>55</v>
+      </c>
+      <c r="D82" t="s">
+        <v>56</v>
+      </c>
       <c r="E82" s="12"/>
       <c r="F82" s="12"/>
       <c r="G82" s="12"/>
@@ -5110,7 +5185,10 @@
       <c r="BP82" s="12"/>
       <c r="BQ82" s="12"/>
     </row>
-    <row r="83" spans="5:69">
+    <row r="83" spans="2:69">
+      <c r="B83" t="s">
+        <v>54</v>
+      </c>
       <c r="E83" s="12"/>
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
@@ -5177,7 +5255,10 @@
       <c r="BP83" s="12"/>
       <c r="BQ83" s="12"/>
     </row>
-    <row r="84" spans="5:69">
+    <row r="84" spans="2:69">
+      <c r="B84" t="s">
+        <v>57</v>
+      </c>
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
       <c r="G84" s="12"/>
@@ -5244,7 +5325,13 @@
       <c r="BP84" s="12"/>
       <c r="BQ84" s="12"/>
     </row>
-    <row r="85" spans="5:69">
+    <row r="85" spans="2:69">
+      <c r="B85" t="s">
+        <v>59</v>
+      </c>
+      <c r="C85" t="s">
+        <v>52</v>
+      </c>
       <c r="E85" s="12"/>
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
@@ -5311,7 +5398,16 @@
       <c r="BP85" s="12"/>
       <c r="BQ85" s="12"/>
     </row>
-    <row r="86" spans="5:69">
+    <row r="86" spans="2:69">
+      <c r="B86" t="s">
+        <v>60</v>
+      </c>
+      <c r="C86" t="s">
+        <v>52</v>
+      </c>
+      <c r="D86" t="s">
+        <v>52</v>
+      </c>
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
@@ -5378,7 +5474,10 @@
       <c r="BP86" s="12"/>
       <c r="BQ86" s="12"/>
     </row>
-    <row r="87" spans="5:69">
+    <row r="87" spans="2:69">
+      <c r="B87" t="s">
+        <v>58</v>
+      </c>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
@@ -5445,7 +5544,16 @@
       <c r="BP87" s="12"/>
       <c r="BQ87" s="12"/>
     </row>
-    <row r="88" spans="5:69">
+    <row r="88" spans="2:69">
+      <c r="B88" t="s">
+        <v>61</v>
+      </c>
+      <c r="C88" t="s">
+        <v>52</v>
+      </c>
+      <c r="D88" t="s">
+        <v>52</v>
+      </c>
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
@@ -5512,7 +5620,13 @@
       <c r="BP88" s="12"/>
       <c r="BQ88" s="12"/>
     </row>
-    <row r="89" spans="5:69">
+    <row r="89" spans="2:69">
+      <c r="B89" t="s">
+        <v>62</v>
+      </c>
+      <c r="C89" t="s">
+        <v>52</v>
+      </c>
       <c r="E89" s="12"/>
       <c r="F89" s="12"/>
       <c r="G89" s="12"/>
@@ -5579,7 +5693,7 @@
       <c r="BP89" s="12"/>
       <c r="BQ89" s="12"/>
     </row>
-    <row r="90" spans="5:69">
+    <row r="90" spans="2:69">
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
@@ -5646,7 +5760,10 @@
       <c r="BP90" s="12"/>
       <c r="BQ90" s="12"/>
     </row>
-    <row r="91" spans="5:69">
+    <row r="91" spans="2:69">
+      <c r="B91" t="s">
+        <v>63</v>
+      </c>
       <c r="E91" s="12"/>
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
@@ -5713,7 +5830,10 @@
       <c r="BP91" s="12"/>
       <c r="BQ91" s="12"/>
     </row>
-    <row r="92" spans="5:69">
+    <row r="92" spans="2:69">
+      <c r="B92" t="s">
+        <v>64</v>
+      </c>
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
@@ -5780,7 +5900,13 @@
       <c r="BP92" s="12"/>
       <c r="BQ92" s="12"/>
     </row>
-    <row r="93" spans="5:69">
+    <row r="93" spans="2:69">
+      <c r="B93" t="s">
+        <v>66</v>
+      </c>
+      <c r="C93" t="s">
+        <v>52</v>
+      </c>
       <c r="E93" s="12"/>
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
@@ -5847,7 +5973,13 @@
       <c r="BP93" s="12"/>
       <c r="BQ93" s="12"/>
     </row>
-    <row r="94" spans="5:69">
+    <row r="94" spans="2:69">
+      <c r="B94" t="s">
+        <v>65</v>
+      </c>
+      <c r="C94" t="s">
+        <v>52</v>
+      </c>
       <c r="E94" s="12"/>
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
@@ -5914,7 +6046,7 @@
       <c r="BP94" s="12"/>
       <c r="BQ94" s="12"/>
     </row>
-    <row r="95" spans="5:69">
+    <row r="95" spans="2:69">
       <c r="E95" s="12"/>
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
@@ -5981,7 +6113,13 @@
       <c r="BP95" s="12"/>
       <c r="BQ95" s="12"/>
     </row>
-    <row r="96" spans="5:69">
+    <row r="96" spans="2:69">
+      <c r="B96" t="s">
+        <v>67</v>
+      </c>
+      <c r="C96" t="s">
+        <v>52</v>
+      </c>
       <c r="E96" s="12"/>
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
@@ -6048,6 +6186,210 @@
       <c r="BP96" s="12"/>
       <c r="BQ96" s="12"/>
     </row>
+    <row r="97" spans="2:69">
+      <c r="B97" t="s">
+        <v>68</v>
+      </c>
+      <c r="C97" t="s">
+        <v>52</v>
+      </c>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
+      <c r="M97" s="12"/>
+      <c r="N97" s="12"/>
+      <c r="O97" s="12"/>
+      <c r="P97" s="12"/>
+      <c r="Q97" s="12"/>
+      <c r="R97" s="12"/>
+      <c r="S97" s="12"/>
+      <c r="T97" s="12"/>
+      <c r="U97" s="12"/>
+      <c r="V97" s="12"/>
+      <c r="W97" s="12"/>
+      <c r="X97" s="12"/>
+      <c r="Y97" s="12"/>
+      <c r="Z97" s="12"/>
+      <c r="AA97" s="12"/>
+      <c r="AB97" s="12"/>
+      <c r="AC97" s="12"/>
+      <c r="AD97" s="12"/>
+      <c r="AE97" s="12"/>
+      <c r="AF97" s="12"/>
+      <c r="AG97" s="12"/>
+      <c r="AH97" s="12"/>
+      <c r="AI97" s="12"/>
+      <c r="AJ97" s="12"/>
+      <c r="AK97" s="12"/>
+      <c r="AL97" s="12"/>
+      <c r="AM97" s="12"/>
+      <c r="AN97" s="12"/>
+      <c r="AO97" s="12"/>
+      <c r="AP97" s="12"/>
+      <c r="AQ97" s="12"/>
+      <c r="AR97" s="12"/>
+      <c r="AS97" s="12"/>
+      <c r="AT97" s="12"/>
+      <c r="AU97" s="12"/>
+      <c r="AV97" s="12"/>
+      <c r="AW97" s="12"/>
+      <c r="AX97" s="12"/>
+      <c r="AY97" s="12"/>
+      <c r="AZ97" s="12"/>
+      <c r="BA97" s="12"/>
+      <c r="BB97" s="12"/>
+      <c r="BC97" s="12"/>
+      <c r="BD97" s="12"/>
+      <c r="BE97" s="12"/>
+      <c r="BF97" s="12"/>
+      <c r="BG97" s="12"/>
+      <c r="BH97" s="12"/>
+      <c r="BI97" s="12"/>
+      <c r="BJ97" s="12"/>
+      <c r="BK97" s="12"/>
+      <c r="BL97" s="12"/>
+      <c r="BM97" s="12"/>
+      <c r="BN97" s="12"/>
+      <c r="BO97" s="12"/>
+      <c r="BP97" s="12"/>
+      <c r="BQ97" s="12"/>
+    </row>
+    <row r="98" spans="2:69">
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="12"/>
+      <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
+      <c r="L98" s="12"/>
+      <c r="M98" s="12"/>
+      <c r="N98" s="12"/>
+      <c r="O98" s="12"/>
+      <c r="P98" s="12"/>
+      <c r="Q98" s="12"/>
+      <c r="R98" s="12"/>
+      <c r="S98" s="12"/>
+      <c r="T98" s="12"/>
+      <c r="U98" s="12"/>
+      <c r="V98" s="12"/>
+      <c r="W98" s="12"/>
+      <c r="X98" s="12"/>
+      <c r="Y98" s="12"/>
+      <c r="Z98" s="12"/>
+      <c r="AA98" s="12"/>
+      <c r="AB98" s="12"/>
+      <c r="AC98" s="12"/>
+      <c r="AD98" s="12"/>
+      <c r="AE98" s="12"/>
+      <c r="AF98" s="12"/>
+      <c r="AG98" s="12"/>
+      <c r="AH98" s="12"/>
+      <c r="AI98" s="12"/>
+      <c r="AJ98" s="12"/>
+      <c r="AK98" s="12"/>
+      <c r="AL98" s="12"/>
+      <c r="AM98" s="12"/>
+      <c r="AN98" s="12"/>
+      <c r="AO98" s="12"/>
+      <c r="AP98" s="12"/>
+      <c r="AQ98" s="12"/>
+      <c r="AR98" s="12"/>
+      <c r="AS98" s="12"/>
+      <c r="AT98" s="12"/>
+      <c r="AU98" s="12"/>
+      <c r="AV98" s="12"/>
+      <c r="AW98" s="12"/>
+      <c r="AX98" s="12"/>
+      <c r="AY98" s="12"/>
+      <c r="AZ98" s="12"/>
+      <c r="BA98" s="12"/>
+      <c r="BB98" s="12"/>
+      <c r="BC98" s="12"/>
+      <c r="BD98" s="12"/>
+      <c r="BE98" s="12"/>
+      <c r="BF98" s="12"/>
+      <c r="BG98" s="12"/>
+      <c r="BH98" s="12"/>
+      <c r="BI98" s="12"/>
+      <c r="BJ98" s="12"/>
+      <c r="BK98" s="12"/>
+      <c r="BL98" s="12"/>
+      <c r="BM98" s="12"/>
+      <c r="BN98" s="12"/>
+      <c r="BO98" s="12"/>
+      <c r="BP98" s="12"/>
+      <c r="BQ98" s="12"/>
+    </row>
+    <row r="99" spans="2:69">
+      <c r="B99" t="s">
+        <v>69</v>
+      </c>
+      <c r="C99" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="100" spans="2:69">
+      <c r="B100" t="s">
+        <v>70</v>
+      </c>
+      <c r="C100" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="101" spans="2:69">
+      <c r="B101" t="s">
+        <v>71</v>
+      </c>
+      <c r="C101" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="104" spans="2:69">
+      <c r="B104" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="105" spans="2:69">
+      <c r="B105" t="s">
+        <v>73</v>
+      </c>
+      <c r="C105" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="106" spans="2:69">
+      <c r="B106" t="s">
+        <v>74</v>
+      </c>
+      <c r="C106" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="109" spans="2:69">
+      <c r="B109" t="s">
+        <v>75</v>
+      </c>
+      <c r="C109" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="111" spans="2:69">
+      <c r="B111" t="s">
+        <v>76</v>
+      </c>
+      <c r="C111" t="s">
+        <v>52</v>
+      </c>
+      <c r="D111" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="http://localhost/snorg/query.php?action=GetFriends&amp;owner=0"/>

</xml_diff>